<commit_message>
added sentiment analysis model
</commit_message>
<xml_diff>
--- a/sample/CourtVerdicts.xlsx
+++ b/sample/CourtVerdicts.xlsx
@@ -529,12 +529,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>העותר,ככל,ש,מערער</t>
+          <t>ככל,ש,העותר,מערער</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -590,12 +590,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>המשיב,על,הוא,את,בתל</t>
+          <t>ההכרעה,מינית,אותה,את,כולל</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -648,12 +648,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>משמעותי,חומר,באת,נוסף,המשיב</t>
+          <t>הצהירה,ב,ההצהרה,כוח,נמחקת</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -732,12 +732,12 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>המאמת,השופט,דרש,שונים,משפחות</t>
+          <t>בקשתה,ברם,השופט,הפנים,מטעמים</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -788,12 +788,12 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>לכך,בהמלצתנו,מן,אי,בו</t>
+          <t>מן,לכך,בו,חזר,צו</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -923,12 +923,12 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>הפרסונאלית,מכוח,והיא,דברינו,נעברה</t>
+          <t>אותנו,מדינה,והנחדלים,וכך,מ</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -1464,12 +1464,12 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>עוסק,בסעיף,וכי,שהופקו,המערער</t>
+          <t>כנספח,אלה,המיסוי,הוא,משפחתו</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>negative</t>
         </is>
       </c>
     </row>
@@ -1522,12 +1522,12 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>ובערעורים,ובמקרה,בסכומים,הערות,אנו</t>
+          <t>כוח,עוד,כי,השאיר,גבוהים</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -1579,12 +1579,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>בהמלצת,שח,טרחת,קדם,עוד</t>
+          <t>אנו,קדם,בהמלצת,שכר,זה</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -1634,12 +1634,12 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>נתייתרה,היא,העתירה,להוצאות,בלא</t>
+          <t>בלא,נתייתרה,העתירה,להוצאות,היא</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -1688,12 +1688,12 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>ללא,העתירה,תימחק,להוצאות,כמבוקש</t>
+          <t>כמבוקש,העתירה,תימחק,ללא,צו</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -1757,12 +1757,12 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>מספר,לא,צלחו,מחליטים,סמכות</t>
+          <t>הפנים,החליט,העותרים,ראש,ההחלטה</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -1831,12 +1831,12 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>הסמכות,מופנית,ג,ועדת,ולמועצה</t>
+          <t>השופט,התקנות,הנזכרת,הבחירה,יש</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -1896,12 +1896,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>מחמת,לסייע,במלחמה,להלן,השופטת</t>
+          <t>למכור,ביקש,ידי,מעבירות,נשק</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -1955,12 +1955,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>ללא,של,כבוד,יועבר,לבקשת</t>
+          <t>החזר,יועבר,הרשם,עניין,צו</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -2044,12 +2044,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>חויבה,מנהיים,את,כחברת,לשלם</t>
+          <t>כדין,בגין,מ,כחברת,דרישה</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -2099,12 +2099,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>מיום,בהודעת,הצורך,נמחק,נוכח</t>
+          <t>האמור,בערעור,נמחק,נוכח,מתייתר</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -2154,7 +2154,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>בנפרד,דוחים,נימוקינו,יינתנו,העתירה</t>
+          <t>דוחים,בנפרד,העתירה,נימוקינו,יינתנו</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -2265,12 +2265,12 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>איתה,הורשע,כולם,ניסיון,על</t>
+          <t>כבוד,משפחה,המערער,וסעיף,בר</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -2326,12 +2326,12 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>נדחית,מונחת,ילדים,תושבות,נוקט</t>
+          <t>נדחית,הופסקו,בעתירה,ואין,לנשים</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -2380,12 +2380,12 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>את,היא,צו,התייתר,להוצאות</t>
+          <t>צו,נמחקת,להחזר,אגרה,התייתר</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -2435,12 +2435,12 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>לבקשת,הבקשה,צו,להחזר,אין</t>
+          <t>צו,העתירה,את,לבקשת,נמחקת</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -2525,12 +2525,12 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>עתה,על,שהייה,–,שנת</t>
+          <t>עיקר,יפוג,יחדשו,עד,במהלך</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -2631,12 +2631,12 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>נגרם,חלק,חד,בחזהו,ס</t>
+          <t>שנים,מאסר,בפועל,של,מדינת</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -2728,12 +2728,12 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>עקב,בחדר,עליו,השופטת,הנקי</t>
+          <t>אחר,והמנוח,דקירה,מאסר,בלבו</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -2788,12 +2788,12 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>והגענו,משא,אי,המחוזי,למסקנה</t>
+          <t>בחנו,התכנון,של,למותר,הדין</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -2858,12 +2858,12 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>בירושלים,השאר,המצדיק,תיגרע,בפרשה</t>
+          <t>לבקשה,השבוע,להשתחרר,ביניים,אזרחיים</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -2931,12 +2931,12 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>המדינה,אם,בעבור,ההתאגדות,להידחות</t>
+          <t>מספר,לרישום,אם,האלף,כינוי</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -2991,12 +2991,12 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>מתקבל,לוי,לתעבורה,לקיים,השופט</t>
+          <t>בעניינו,השופט,עמדת,בית,ופסקי</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -3140,12 +3140,12 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>מלדון,במקביל,לבית,הינו,המחוזי</t>
+          <t>הגיש,בית,התביעה,בניגוד,היכן</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -3194,12 +3194,12 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>בין,משפטי,בעלי,מתנהל,שנים</t>
+          <t>שנים,זה,בעלי,בין,משפטי</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -3252,12 +3252,12 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>עא,הרשם,על,כב,הוגש</t>
+          <t>וערעור,להגיש,מיום,קבע,מרזל</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -3325,12 +3325,12 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>חודשי,הוכחה,בעבירות,האמורות,בגזר</t>
+          <t>מסוכן,בא,החזקת,חומרתן,זה</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -3382,12 +3382,12 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>הדין,צו,המשפט,להוצאות,של</t>
+          <t>צו,המשפט,מבוטלים,המחוזי,בית</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -3451,12 +3451,12 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>בתיק,בעונש,ובעקבות,כמו,עתרה</t>
+          <t>עצמית,למערער,עליו,למשך,זה</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -3506,12 +3506,12 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>הרבני,לתיקון,העותר,של,אביב</t>
+          <t>לבית,האזורי,בתל,בקשה,הגיש</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -3564,12 +3564,12 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>כמה,תחושה,כל,הערעור,מקרה</t>
+          <t>על,עד,לפנינו,מקרה,כלפיו</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -3660,12 +3660,12 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>בסלילת,מתנהל,מיום,ישראל,והנוגע</t>
+          <t>במשרד,שנים,מחש,במשטרת,אין</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -3753,12 +3753,12 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>מקום,מ,כן,הוא,עדיין</t>
+          <t>שוחרר,המערער,עונש,שתי,לשנים</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -3831,12 +3831,12 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>לסעיף,הועברו,נתונה,חידוש,השר</t>
+          <t>יחדש,ברשות,ששה,חידוש,הרכב</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
     </row>
@@ -3899,12 +3899,12 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>ביום,הזמנים,נחתמו,עליהם,התקנות</t>
+          <t>של,הגמל,קשר,טוענים,הכרח</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
     </row>

</xml_diff>